<commit_message>
more work on renovation modeling, not good enough yet though
</commit_message>
<xml_diff>
--- a/Data/cleaned_and_combined_data/Energy_Intensity/Energy_intensity_constants.xlsx
+++ b/Data/cleaned_and_combined_data/Energy_Intensity/Energy_intensity_constants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annakalesnikavathestrongest/Desktop/NTNUsemester2/TEP4290/Project/TEP4290_project/TEP4290_project/Energy intensity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/954e9104582efe7e/Documents/Python/TEP4290_project/data/cleaned_and_combined_data/Energy_Intensity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98BAFD3-1E3A-674E-BFAF-1E7976CD6DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{D98BAFD3-1E3A-674E-BFAF-1E7976CD6DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5D63C26-313D-4465-943F-A71FB98A4116}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="740" windowWidth="29400" windowHeight="17280" xr2:uid="{C3FE58EA-78F5-5C46-A3D2-3B2AA9A48CB8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C3FE58EA-78F5-5C46-A3D2-3B2AA9A48CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,12 +108,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -180,15 +186,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -209,9 +222,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,7 +262,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -355,7 +368,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -497,7 +510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -507,18 +520,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10331A8-B000-7E40-85D5-55D38F9A886F}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,694 +545,710 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="7">
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7">
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="7">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7">
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="7">
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7">
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="C17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7">
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="3">
+      <c r="C20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7">
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="7">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="4"/>
+      <c r="B23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="3">
+      <c r="C23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="7">
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="7">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="C26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="7">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="7">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="3">
+      <c r="C29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="7">
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="7">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="3">
+      <c r="C32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="7">
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="7">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="4"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="3">
+      <c r="C35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="7">
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="4"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="7">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="4"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="7">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3">
+      <c r="C38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="7">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="4"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="7">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="4"/>
+      <c r="B41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="3">
+      <c r="C41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="7">
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="4"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="7">
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="4"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="7">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="4"/>
+      <c r="B44" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="3">
+      <c r="C44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="7">
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="4"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="7">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="4"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="7">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="3">
+      <c r="C47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="7">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="4"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="4"/>
+      <c r="B50" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="3">
+      <c r="C50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="7">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="4"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="7">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="4"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="4"/>
+      <c r="B53" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="3">
+      <c r="C53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="7">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="4"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="4"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="7">
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="3">
+      <c r="C56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="7">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="4"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="4"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="4"/>
+      <c r="B59" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="3">
+      <c r="C59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="7">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="4"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="4"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="2">
         <v>88.9</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="2">
         <v>49.8</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D64" s="3">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A29:A37"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B37"/>
     <mergeCell ref="A56:A64"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="B59:B61"/>
@@ -1232,22 +1261,6 @@
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="B53:B55"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
calibration of energy use modeling by renovation level
</commit_message>
<xml_diff>
--- a/Data/cleaned_and_combined_data/Energy_Intensity/Energy_intensity_constants.xlsx
+++ b/Data/cleaned_and_combined_data/Energy_Intensity/Energy_intensity_constants.xlsx
@@ -193,14 +193,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -520,7 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10331A8-B000-7E40-85D5-55D38F9A886F}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
@@ -546,662 +546,662 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5">
         <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6">
         <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6">
         <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6">
         <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6">
         <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
         <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6">
         <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="6">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="7">
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6">
         <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="C18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="6">
         <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="8"/>
-      <c r="C19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7">
+      <c r="C20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6">
         <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="7">
+      <c r="C21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="6">
         <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="7">
+      <c r="C22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="6">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="C23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6">
         <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="7">
+      <c r="C24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="6">
         <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="7">
+      <c r="C25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="6">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="7">
+      <c r="C26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6">
         <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="7">
+      <c r="C27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="6">
         <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="7">
+      <c r="C28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="6">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="7">
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6">
         <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="7">
+      <c r="C30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="6">
         <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="7">
+      <c r="C31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="6">
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="4"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="7">
+      <c r="C32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="6">
         <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="4"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="7">
+      <c r="C33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="6">
         <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="4"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="8"/>
-      <c r="C34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="7">
+      <c r="C34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="6">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="7">
+      <c r="C35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="6">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="7">
+      <c r="C36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="6">
         <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="4"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="8"/>
-      <c r="C37" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="7">
+      <c r="C37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="6">
         <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="7">
+      <c r="C38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="6">
         <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="8"/>
-      <c r="C39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="7">
+      <c r="C39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="6">
         <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="4"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="8"/>
-      <c r="C40" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="7">
+      <c r="C40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="6">
         <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="4"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="7">
+      <c r="C41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="6">
         <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="4"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="8"/>
-      <c r="C42" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="7">
+      <c r="C42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="6">
         <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="4"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="8"/>
-      <c r="C43" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="7">
+      <c r="C43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="6">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="4"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="7">
+      <c r="C44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="6">
         <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="4"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="8"/>
-      <c r="C45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="7">
+      <c r="C45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="6">
         <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
+      <c r="A46" s="7"/>
       <c r="B46" s="8"/>
-      <c r="C46" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="7">
+      <c r="C46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="6">
         <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="7">
+      <c r="C47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="6">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="4"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="8"/>
-      <c r="C48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="7">
+      <c r="C48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="4"/>
+      <c r="A49" s="7"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="7">
+      <c r="C49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="6">
         <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="4"/>
+      <c r="A50" s="7"/>
       <c r="B50" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="7">
+      <c r="C50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="6">
         <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="4"/>
+      <c r="A51" s="7"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="7">
+      <c r="C51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="6">
         <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="4"/>
+      <c r="A52" s="7"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="7">
+      <c r="C52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="6">
         <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="4"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="7">
+      <c r="C53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="6">
         <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="4"/>
+      <c r="A54" s="7"/>
       <c r="B54" s="8"/>
-      <c r="C54" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="7">
+      <c r="C54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="6">
         <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="4"/>
+      <c r="A55" s="7"/>
       <c r="B55" s="8"/>
-      <c r="C55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="7">
+      <c r="C55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="7">
+      <c r="C56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="6">
         <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="4"/>
+      <c r="A57" s="7"/>
       <c r="B57" s="8"/>
-      <c r="C57" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="7">
+      <c r="C57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="6">
         <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="4"/>
+      <c r="A58" s="7"/>
       <c r="B58" s="8"/>
-      <c r="C58" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="7">
+      <c r="C58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="4"/>
+      <c r="A59" s="7"/>
       <c r="B59" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="7">
+      <c r="C59" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="6">
         <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="4"/>
+      <c r="A60" s="7"/>
       <c r="B60" s="8"/>
-      <c r="C60" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="7">
+      <c r="C60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="6">
         <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
+      <c r="A61" s="7"/>
       <c r="B61" s="8"/>
-      <c r="C61" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="7">
+      <c r="C61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4" t="s">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -1212,8 +1212,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
       <c r="C63" s="1" t="s">
         <v>6</v>
       </c>
@@ -1222,8 +1222,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
       <c r="C64" s="1" t="s">
         <v>7</v>
       </c>
@@ -1233,22 +1233,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B37"/>
     <mergeCell ref="A56:A64"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="B59:B61"/>
@@ -1261,6 +1245,22 @@
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="B53:B55"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A29:A37"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>